<commit_message>
use die symbol in Pig GUI impact game added (in progress)
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ECBCBA-C406-4DA9-8B97-0A172DB36B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B4176A-67E0-44D8-A7E1-4C1CAA0EAE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="185">
   <si>
     <t>Pig</t>
   </si>
@@ -172,12 +172,6 @@
     <t>https://boardgamegeek.com/boardgame/3886/nine-mens-morris</t>
   </si>
   <si>
-    <t>Strike</t>
-  </si>
-  <si>
-    <t>https://boardgamegeek.com/boardgame/123570/strike</t>
-  </si>
-  <si>
     <t>https://boardgamegeek.com/boardgame/220988/criss-cross</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t>https://boardgamegeek.com/boardgame/2731/upthrust</t>
   </si>
   <si>
-    <t>Farmer finance</t>
-  </si>
-  <si>
     <t>https://boardgamegeek.com/boardgame/201028/farmers-finances</t>
   </si>
   <si>
@@ -556,9 +547,6 @@
     <t>graphs</t>
   </si>
   <si>
-    <t>basic structures</t>
-  </si>
-  <si>
     <t>arrays, algorithms</t>
   </si>
   <si>
@@ -566,13 +554,55 @@
   </si>
   <si>
     <t>Cards</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/246228/impact-battle-elements</t>
+  </si>
+  <si>
+    <t>https://whatsericplaying.com/2018/12/24/impact-battle-of-elements/</t>
+  </si>
+  <si>
+    <t>Twin win</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/31711/twin-win</t>
+  </si>
+  <si>
+    <t>basic elements</t>
+  </si>
+  <si>
+    <t>Farmers Finances</t>
+  </si>
+  <si>
+    <t>farmers</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/thread/1525550/farmers-finances-2016-9-card-nanogame-contest</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>orchard</t>
+  </si>
+  <si>
+    <t>https://www.sideroomgames.com/product/orchard/</t>
+  </si>
+  <si>
+    <t>http://www.nestorgames.com/hippos_l.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,6 +615,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -654,8 +691,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:J8" totalsRowShown="0">
-  <autoFilter ref="A1:J8" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0">
+  <autoFilter ref="A1:J11" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A79D0D46-4EBF-4D48-8DFC-C1F9B9F5B13B}" name="Name"/>
     <tableColumn id="10" xr3:uid="{0B874210-D71E-4787-AC57-435630C4FB1F}" name="Folder"/>
@@ -979,15 +1016,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA158D42-EF44-4D25-B732-21E60DAA7307}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
@@ -1002,31 +1039,31 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" t="s">
         <v>104</v>
-      </c>
-      <c r="F1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1034,7 +1071,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1049,31 +1086,31 @@
         <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H2" s="5">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E3">
         <v>5.9</v>
@@ -1082,31 +1119,31 @@
         <v>50</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H3" s="5">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E4">
         <v>5.0999999999999996</v>
@@ -1115,31 +1152,31 @@
         <v>100</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E5">
         <v>6.1</v>
@@ -1148,31 +1185,31 @@
         <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6">
         <v>7.1</v>
@@ -1181,16 +1218,16 @@
         <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="L6" s="3"/>
     </row>
@@ -1199,13 +1236,13 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E7">
         <v>6.1</v>
@@ -1214,31 +1251,31 @@
         <v>50</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H7" s="5">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8">
         <v>6.7</v>
@@ -1247,25 +1284,106 @@
         <v>100</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J8" t="s">
+      <c r="D9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9">
+        <v>6.7</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="I9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10">
+        <v>6.3</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="I10" t="s">
         <v>170</v>
       </c>
-      <c r="L8" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11">
+        <v>7.4</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I11" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I48 I50:I1048576" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
       <formula1>Categories_Range</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G48" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8 G10:G48" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
       <formula1>"Low,High"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1283,41 +1401,47 @@
     <hyperlink ref="D7" r:id="rId11" xr:uid="{D6CE8703-8F93-4882-BEFD-866FA986BE7E}"/>
     <hyperlink ref="C8" r:id="rId12" xr:uid="{9CCF4779-4997-4826-B069-ED6AF8CD3D91}"/>
     <hyperlink ref="D8" r:id="rId13" xr:uid="{31A51631-0C88-4ABC-87FE-D5DBD5DA9A3D}"/>
+    <hyperlink ref="C9" r:id="rId14" xr:uid="{E751E88E-5FF3-4FFC-A298-C92A80243714}"/>
+    <hyperlink ref="C10" r:id="rId15" xr:uid="{776CBF58-DDF1-4EF3-8413-F4CA801CDCC7}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{513AA72A-9CF0-4130-AF38-4E77D16460D1}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{E327BEBE-F953-42C1-8769-F8E5CD69EB9C}"/>
+    <hyperlink ref="C11" r:id="rId18" xr:uid="{C02C3B6A-9987-4C26-9285-2B118139009F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A9A40E-25F0-458E-A251-DF2D64A47FEF}">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1328,19 +1452,19 @@
         <v>6.3</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1351,13 +1475,13 @@
         <v>5.6</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" t="s">
         <v>155</v>
       </c>
-      <c r="J3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1368,13 +1492,13 @@
         <v>6.8</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1385,16 +1509,16 @@
         <v>6.4</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" t="s">
         <v>155</v>
       </c>
-      <c r="J5" t="s">
-        <v>158</v>
-      </c>
       <c r="L5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1405,16 +1529,16 @@
         <v>6.6</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" t="s">
         <v>159</v>
       </c>
-      <c r="J6" t="s">
-        <v>160</v>
-      </c>
-      <c r="L6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1425,15 +1549,15 @@
         <v>6.5</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>31</v>
@@ -1442,15 +1566,15 @@
         <v>7</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>32</v>
@@ -1459,16 +1583,16 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1479,628 +1603,623 @@
         <v>5.3</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11">
-        <v>6.9</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="J11" t="s">
-        <v>95</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H12">
         <v>6.4</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H13">
         <v>6.2</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H14">
         <v>6.6</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H15">
         <v>6.3</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+      <c r="M15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16">
         <v>6.1</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H17">
         <v>6.3</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H18">
         <v>6.3</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H19">
         <v>6.7</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H20">
         <v>6</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H21">
         <v>7.4</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H22">
         <v>6.8</v>
       </c>
       <c r="J22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>137</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H23">
-        <v>6.3</v>
-      </c>
-      <c r="J23" t="s">
-        <v>164</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>166</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H24">
         <v>6.8</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H25">
         <v>6.9</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H26">
         <v>6.2</v>
       </c>
       <c r="J26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="1"/>
-      <c r="L27" s="7"/>
+      <c r="A27" t="s">
+        <v>175</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27">
+        <v>6.3</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="L28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="L29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J33" t="s">
-        <v>97</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>65</v>
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J35" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>103</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D49">
+      <c r="D51">
         <v>6.4</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F51" t="s">
         <v>5</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G51" t="s">
         <v>10</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H51" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>126</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>135</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>141</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>142</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>147</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>16</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F49" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F51" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
       <formula1>"Low,High"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H49" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H51" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
       <formula1>Categories_Range</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8E64C7A1-5801-4044-B589-D487C836BFCF}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{8E059295-B16B-4E97-8E60-ED1DE5F2307D}"/>
-    <hyperlink ref="B68" r:id="rId3" xr:uid="{7BEC1253-D118-4590-AF24-CDE738F8B1D8}"/>
+    <hyperlink ref="B70" r:id="rId3" xr:uid="{7BEC1253-D118-4590-AF24-CDE738F8B1D8}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{9B7928A1-3A7E-46CC-AA5A-B57923DDFA32}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{ADADF905-ABC1-4EF5-BE7E-E10F199DD469}"/>
     <hyperlink ref="B6" r:id="rId6" xr:uid="{1BC6A08D-1D08-4623-8C82-B71A0592AAB6}"/>
     <hyperlink ref="B7" r:id="rId7" xr:uid="{852CA370-9A08-4A1C-B844-C12255B3943D}"/>
     <hyperlink ref="B8" r:id="rId8" xr:uid="{E666E340-63E8-4663-948F-406098389801}"/>
     <hyperlink ref="B9" r:id="rId9" xr:uid="{4C6A5B99-F01F-4E74-84FF-89478DB73084}"/>
-    <hyperlink ref="B29" r:id="rId10" xr:uid="{6F79CD7B-678A-4274-89B4-B9544BE83041}"/>
-    <hyperlink ref="B30" r:id="rId11" xr:uid="{9211F0DC-E5BA-4E37-8711-10B29744A713}"/>
-    <hyperlink ref="B31" r:id="rId12" xr:uid="{44B7F867-AC69-4A22-83B6-46E52511ACAE}"/>
-    <hyperlink ref="B32" r:id="rId13" xr:uid="{F4B22872-BE08-49A5-9D25-B40B43B58B00}"/>
-    <hyperlink ref="B10" r:id="rId14" xr:uid="{ADB09910-F42D-4F20-A4F2-76CF9D12AED9}"/>
-    <hyperlink ref="B11" r:id="rId15" xr:uid="{88DF76A4-C68B-4703-B981-344E449C6D62}"/>
-    <hyperlink ref="B12" r:id="rId16" xr:uid="{D8FD9E36-7834-451C-BCEA-39AEBB29495C}"/>
-    <hyperlink ref="B13" r:id="rId17" xr:uid="{D415E350-C5ED-4B12-9A8A-72DFD905618E}"/>
-    <hyperlink ref="B33" r:id="rId18" xr:uid="{2DE0CFB5-2C9F-4FF0-AAD0-15FADBF567E0}"/>
-    <hyperlink ref="B14" r:id="rId19" xr:uid="{9CCFFBB9-3B72-4FB7-94F3-1C8439CA8D47}"/>
-    <hyperlink ref="B15" r:id="rId20" xr:uid="{5C9F6E2F-3112-48A6-B5B3-72043F9FA591}"/>
-    <hyperlink ref="B16" r:id="rId21" xr:uid="{DDFD90C3-8BF5-4CA2-96A4-256D35D2D59E}"/>
-    <hyperlink ref="B28" r:id="rId22" xr:uid="{7598335B-1BBA-46B0-B82C-77CC49C095EF}"/>
-    <hyperlink ref="B17" r:id="rId23" xr:uid="{8C5DB89C-A095-4851-A83C-C1AEE9B102F4}"/>
-    <hyperlink ref="B18" r:id="rId24" xr:uid="{D29184C3-5D1A-443B-9B34-4C4114F1E387}"/>
-    <hyperlink ref="B19" r:id="rId25" xr:uid="{DE020276-739E-4605-82CA-4152C2825027}"/>
-    <hyperlink ref="B37" r:id="rId26" xr:uid="{5A0FEA15-888C-4075-9C2F-CFD8546985A7}"/>
-    <hyperlink ref="B38" r:id="rId27" xr:uid="{2C05C520-6C02-4D0C-BB87-EEDF41E33FC8}"/>
-    <hyperlink ref="B39" r:id="rId28" xr:uid="{A827F7CF-12E3-44AE-BBD1-1A9A96F3FB02}"/>
-    <hyperlink ref="B40" r:id="rId29" xr:uid="{A1A4F6A6-F4E7-42AF-B52D-3A521F5406E5}"/>
-    <hyperlink ref="B20" r:id="rId30" xr:uid="{28FFB9B7-2753-4040-946E-FF2B9EA9EC0B}"/>
-    <hyperlink ref="B42" r:id="rId31" xr:uid="{FE39472A-D9C9-4EF0-AEBC-06F8FF1443E7}"/>
-    <hyperlink ref="B43" r:id="rId32" xr:uid="{1108D29F-FA18-4293-B305-A0EF22F38E43}"/>
-    <hyperlink ref="B46" r:id="rId33" xr:uid="{BD40941F-3476-49F4-A2FE-4355F43FFB72}"/>
-    <hyperlink ref="B47" r:id="rId34" xr:uid="{48489DD5-0C1A-4332-ADD5-32201C6C680E}"/>
-    <hyperlink ref="B49" r:id="rId35" xr:uid="{D62D0431-7742-493B-B009-421431FDA2F8}"/>
-    <hyperlink ref="C49" r:id="rId36" xr:uid="{A223641B-2ACC-4C7E-ADA9-114B861ED482}"/>
-    <hyperlink ref="B21" r:id="rId37" xr:uid="{4C456AD6-F8A4-4F50-BB13-B45ADB92D416}"/>
-    <hyperlink ref="B53" r:id="rId38" xr:uid="{0E8C2D49-C640-4491-A333-E7657B4A3672}"/>
-    <hyperlink ref="B54" r:id="rId39" xr:uid="{75E85909-D109-431E-9850-DDF0148E901E}"/>
-    <hyperlink ref="B22" r:id="rId40" xr:uid="{5E39EF7D-055F-4DB2-BB3B-A0F841DB8313}"/>
-    <hyperlink ref="B56" r:id="rId41" xr:uid="{13E723D6-1FD1-4E3C-A566-3BBB021EE312}"/>
-    <hyperlink ref="B57" r:id="rId42" xr:uid="{26A32048-9EC8-4145-AB5D-8A9AB962E3BF}"/>
-    <hyperlink ref="B23" r:id="rId43" xr:uid="{A0327004-F52F-466F-BEB6-79137BB3CCEC}"/>
-    <hyperlink ref="B24" r:id="rId44" xr:uid="{20635745-E571-4992-9762-4A7AF1CE514E}"/>
-    <hyperlink ref="B61" r:id="rId45" xr:uid="{0245698D-0017-4BE5-BA95-484935FE4171}"/>
-    <hyperlink ref="B25" r:id="rId46" xr:uid="{F3942003-110E-425E-A163-21049FB9CB8F}"/>
-    <hyperlink ref="B63" r:id="rId47" xr:uid="{D2FED77C-07F4-432A-9101-560A5C83BEB5}"/>
-    <hyperlink ref="B64" r:id="rId48" xr:uid="{91E3AA44-1161-40E0-A15C-324284007D73}"/>
-    <hyperlink ref="B65" r:id="rId49" xr:uid="{E5D8CB8A-64AD-48E3-A774-63A0FA6EA437}"/>
-    <hyperlink ref="B26" r:id="rId50" xr:uid="{7C42C010-5880-480F-AA12-C5D610003B9E}"/>
-    <hyperlink ref="B44" r:id="rId51" xr:uid="{5A6573CB-BC16-4292-801B-D3EC4C9D3130}"/>
-    <hyperlink ref="B45" r:id="rId52" xr:uid="{E6BEA243-9351-4DF7-B6D2-70D9924B0513}"/>
+    <hyperlink ref="B31" r:id="rId10" xr:uid="{6F79CD7B-678A-4274-89B4-B9544BE83041}"/>
+    <hyperlink ref="B32" r:id="rId11" xr:uid="{9211F0DC-E5BA-4E37-8711-10B29744A713}"/>
+    <hyperlink ref="B33" r:id="rId12" xr:uid="{44B7F867-AC69-4A22-83B6-46E52511ACAE}"/>
+    <hyperlink ref="B34" r:id="rId13" xr:uid="{F4B22872-BE08-49A5-9D25-B40B43B58B00}"/>
+    <hyperlink ref="B12" r:id="rId14" xr:uid="{D8FD9E36-7834-451C-BCEA-39AEBB29495C}"/>
+    <hyperlink ref="B13" r:id="rId15" xr:uid="{D415E350-C5ED-4B12-9A8A-72DFD905618E}"/>
+    <hyperlink ref="B35" r:id="rId16" xr:uid="{2DE0CFB5-2C9F-4FF0-AAD0-15FADBF567E0}"/>
+    <hyperlink ref="B14" r:id="rId17" xr:uid="{9CCFFBB9-3B72-4FB7-94F3-1C8439CA8D47}"/>
+    <hyperlink ref="B15" r:id="rId18" xr:uid="{5C9F6E2F-3112-48A6-B5B3-72043F9FA591}"/>
+    <hyperlink ref="B16" r:id="rId19" xr:uid="{DDFD90C3-8BF5-4CA2-96A4-256D35D2D59E}"/>
+    <hyperlink ref="B30" r:id="rId20" xr:uid="{7598335B-1BBA-46B0-B82C-77CC49C095EF}"/>
+    <hyperlink ref="B17" r:id="rId21" xr:uid="{8C5DB89C-A095-4851-A83C-C1AEE9B102F4}"/>
+    <hyperlink ref="B18" r:id="rId22" xr:uid="{D29184C3-5D1A-443B-9B34-4C4114F1E387}"/>
+    <hyperlink ref="B19" r:id="rId23" xr:uid="{DE020276-739E-4605-82CA-4152C2825027}"/>
+    <hyperlink ref="B39" r:id="rId24" xr:uid="{5A0FEA15-888C-4075-9C2F-CFD8546985A7}"/>
+    <hyperlink ref="B40" r:id="rId25" xr:uid="{2C05C520-6C02-4D0C-BB87-EEDF41E33FC8}"/>
+    <hyperlink ref="B41" r:id="rId26" xr:uid="{A827F7CF-12E3-44AE-BBD1-1A9A96F3FB02}"/>
+    <hyperlink ref="B42" r:id="rId27" xr:uid="{A1A4F6A6-F4E7-42AF-B52D-3A521F5406E5}"/>
+    <hyperlink ref="B20" r:id="rId28" xr:uid="{28FFB9B7-2753-4040-946E-FF2B9EA9EC0B}"/>
+    <hyperlink ref="B44" r:id="rId29" xr:uid="{FE39472A-D9C9-4EF0-AEBC-06F8FF1443E7}"/>
+    <hyperlink ref="B45" r:id="rId30" xr:uid="{1108D29F-FA18-4293-B305-A0EF22F38E43}"/>
+    <hyperlink ref="B48" r:id="rId31" xr:uid="{BD40941F-3476-49F4-A2FE-4355F43FFB72}"/>
+    <hyperlink ref="B49" r:id="rId32" xr:uid="{48489DD5-0C1A-4332-ADD5-32201C6C680E}"/>
+    <hyperlink ref="B51" r:id="rId33" xr:uid="{D62D0431-7742-493B-B009-421431FDA2F8}"/>
+    <hyperlink ref="C51" r:id="rId34" xr:uid="{A223641B-2ACC-4C7E-ADA9-114B861ED482}"/>
+    <hyperlink ref="B21" r:id="rId35" xr:uid="{4C456AD6-F8A4-4F50-BB13-B45ADB92D416}"/>
+    <hyperlink ref="B55" r:id="rId36" xr:uid="{0E8C2D49-C640-4491-A333-E7657B4A3672}"/>
+    <hyperlink ref="B56" r:id="rId37" xr:uid="{75E85909-D109-431E-9850-DDF0148E901E}"/>
+    <hyperlink ref="B22" r:id="rId38" xr:uid="{5E39EF7D-055F-4DB2-BB3B-A0F841DB8313}"/>
+    <hyperlink ref="B58" r:id="rId39" xr:uid="{13E723D6-1FD1-4E3C-A566-3BBB021EE312}"/>
+    <hyperlink ref="B59" r:id="rId40" xr:uid="{26A32048-9EC8-4145-AB5D-8A9AB962E3BF}"/>
+    <hyperlink ref="B24" r:id="rId41" xr:uid="{20635745-E571-4992-9762-4A7AF1CE514E}"/>
+    <hyperlink ref="B63" r:id="rId42" xr:uid="{0245698D-0017-4BE5-BA95-484935FE4171}"/>
+    <hyperlink ref="B25" r:id="rId43" xr:uid="{F3942003-110E-425E-A163-21049FB9CB8F}"/>
+    <hyperlink ref="B65" r:id="rId44" xr:uid="{D2FED77C-07F4-432A-9101-560A5C83BEB5}"/>
+    <hyperlink ref="B66" r:id="rId45" xr:uid="{91E3AA44-1161-40E0-A15C-324284007D73}"/>
+    <hyperlink ref="B67" r:id="rId46" xr:uid="{E5D8CB8A-64AD-48E3-A774-63A0FA6EA437}"/>
+    <hyperlink ref="B26" r:id="rId47" xr:uid="{7C42C010-5880-480F-AA12-C5D610003B9E}"/>
+    <hyperlink ref="B46" r:id="rId48" xr:uid="{5A6573CB-BC16-4292-801B-D3EC4C9D3130}"/>
+    <hyperlink ref="B47" r:id="rId49" xr:uid="{E6BEA243-9351-4DF7-B6D2-70D9924B0513}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId50"/>
 </worksheet>
 </file>
 
@@ -2119,22 +2238,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pokerdice: bugfixes, updated instructions
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B4176A-67E0-44D8-A7E1-4C1CAA0EAE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82CE5D8-6D78-4ECE-97B5-5D716F217976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA158D42-EF44-4D25-B732-21E60DAA7307}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A9A40E-25F0-458E-A251-DF2D64A47FEF}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
minor improvements; no thanks! rules added
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EAD665-FCDC-4573-875B-B4F87E7A90A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A2BEB2-EE44-4105-B82F-53A93405F5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1236,7 +1236,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>122</v>
@@ -1432,11 +1432,12 @@
     <hyperlink ref="D10" r:id="rId16" xr:uid="{513AA72A-9CF0-4130-AF38-4E77D16460D1}"/>
     <hyperlink ref="D11" r:id="rId17" xr:uid="{E327BEBE-F953-42C1-8769-F8E5CD69EB9C}"/>
     <hyperlink ref="C11" r:id="rId18" xr:uid="{C02C3B6A-9987-4C26-9285-2B118139009F}"/>
+    <hyperlink ref="D6" r:id="rId19" xr:uid="{BE718736-4E6D-47AC-9AF1-9A2048A1D488}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId20"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
othello: message box fixed, rules added
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A2BEB2-EE44-4105-B82F-53A93405F5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39759D5D-1CA4-414C-9D5D-7CC4A66ECD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Impact reworked, documentation added; paletto readme added
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84304ED0-9540-42AA-9912-4CA6B30DB80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72E8130-ED7B-41B1-AE07-9902A30D6870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -1058,7 +1058,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Farmers finances refactoring and documentation
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72E8130-ED7B-41B1-AE07-9902A30D6870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BEFD50-22F5-42C9-BBA1-CFE68318F8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -19,7 +19,8 @@
     <sheet name="CS Topics" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Categories_Range">Categories_Table[Category]</definedName>
+    <definedName name="Categories_Range">Table_1[Category]</definedName>
+    <definedName name="Topics_Range">Table3[Topic]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="216">
   <si>
     <t>Pig</t>
   </si>
@@ -331,12 +332,6 @@
     <t>Abstract Strategy</t>
   </si>
   <si>
-    <t>2d arrays</t>
-  </si>
-  <si>
-    <t>arrays</t>
-  </si>
-  <si>
     <t>https://boardgamegeek.com/boardgame/204583/kingdomino</t>
   </si>
   <si>
@@ -352,12 +347,6 @@
     <t>BGG Rating</t>
   </si>
   <si>
-    <t>GUI value</t>
-  </si>
-  <si>
-    <t>CS topics</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -544,15 +533,6 @@
     <t>Yahtzee</t>
   </si>
   <si>
-    <t>graphs</t>
-  </si>
-  <si>
-    <t>arrays, algorithms</t>
-  </si>
-  <si>
-    <t>Strategy</t>
-  </si>
-  <si>
     <t>Cards</t>
   </si>
   <si>
@@ -574,9 +554,6 @@
     <t>https://boardgamegeek.com/boardgame/31711/twin-win</t>
   </si>
   <si>
-    <t>basic elements</t>
-  </si>
-  <si>
     <t>Farmers Finances</t>
   </si>
   <si>
@@ -635,6 +612,84 @@
   </si>
   <si>
     <t>https://boardgamegeek.com/blogpost/125328/family-inc-diamonds-are-gamblers-best-friend</t>
+  </si>
+  <si>
+    <t>GUI Value</t>
+  </si>
+  <si>
+    <t>https://buttonshygames.com</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/239938/kintsugi</t>
+  </si>
+  <si>
+    <t>Kintsugi</t>
+  </si>
+  <si>
+    <t>Pentomino</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/43411/pentomino</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/21730/delta</t>
+  </si>
+  <si>
+    <t>Cat tower</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/275857/cat-tower</t>
+  </si>
+  <si>
+    <t>Pocket boxing</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/168577/pocket-sports-boxing</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/329873/grove-9-card-solitaire-game</t>
+  </si>
+  <si>
+    <t>Grove</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Basics</t>
+  </si>
+  <si>
+    <t>Algorithms</t>
+  </si>
+  <si>
+    <t>Algorithms+</t>
+  </si>
+  <si>
+    <t>2D Arrays</t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Topic1</t>
+  </si>
+  <si>
+    <t>Topic2</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Gongor Whist</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/64520/gongor-whist</t>
   </si>
 </sst>
 </file>
@@ -730,29 +785,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0">
-  <autoFilter ref="A1:J11" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K11" totalsRowShown="0">
+  <autoFilter ref="A1:K11" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A79D0D46-4EBF-4D48-8DFC-C1F9B9F5B13B}" name="Name"/>
     <tableColumn id="10" xr3:uid="{0B874210-D71E-4787-AC57-435630C4FB1F}" name="Folder"/>
     <tableColumn id="2" xr3:uid="{C7E7642E-11A0-483D-B932-568C3B4D13E7}" name="BGG" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{A66580A4-763E-4CD1-8E82-0C78FCB85B3F}" name="AltLink" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" xr3:uid="{2F0C60EF-78A8-4458-8C7B-4793A7EE120D}" name="BGG Rating"/>
     <tableColumn id="5" xr3:uid="{CD7AF3C2-1E8E-41CD-B153-7B602A44CED7}" name="Core LOC"/>
-    <tableColumn id="6" xr3:uid="{150FDA9B-53B3-42B7-90F7-716F00F5F2E1}" name="GUI value" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{150FDA9B-53B3-42B7-90F7-716F00F5F2E1}" name="GUI Value" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{D87C9AC2-F6D9-4420-9F6C-520990E39ED3}" name="Players" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{8C97285A-61DF-4233-8ED8-21EE1A66F694}" name="Category"/>
-    <tableColumn id="9" xr3:uid="{941B7D52-3C55-47A4-8A01-F9FD1125ACF5}" name="CS topics"/>
+    <tableColumn id="12" xr3:uid="{4938E1A0-094E-4AA3-9D6F-6D772BAFCD11}" name="Topic1"/>
+    <tableColumn id="9" xr3:uid="{941B7D52-3C55-47A4-8A01-F9FD1125ACF5}" name="Topic2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEE554B1-F67F-4ABA-8798-288D364C4F45}" name="Categories_Table" displayName="Categories_Table" ref="A1:A5" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEE554B1-F67F-4ABA-8798-288D364C4F45}" name="Table_1" displayName="Table_1" ref="A1:A5" totalsRowShown="0">
   <autoFilter ref="A1:A5" xr:uid="{DEE554B1-F67F-4ABA-8798-288D364C4F45}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{BFDF39EE-9E9B-4819-B5CA-97A2D84CFF08}" name="Category"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5A4F6B6-883A-4614-990C-71A7CFEE37F6}" name="Table3" displayName="Table3" ref="A1:A7" totalsRowShown="0">
+  <autoFilter ref="A1:A7" xr:uid="{B5A4F6B6-883A-4614-990C-71A7CFEE37F6}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{72E2FC71-0297-4991-865E-8F5B57FF45F5}" name="Topic"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1055,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA158D42-EF44-4D25-B732-21E60DAA7307}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,48 +1135,53 @@
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
         <v>86</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>190</v>
       </c>
       <c r="H1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I1" t="s">
         <v>94</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="K1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1125,7 +1196,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H2" s="5">
         <v>2</v>
@@ -1134,16 +1205,16 @@
         <v>93</v>
       </c>
       <c r="J2" t="s">
-        <v>177</v>
-      </c>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>64</v>
@@ -1158,25 +1229,25 @@
         <v>50</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H3" s="5">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="J3" t="s">
-        <v>97</v>
-      </c>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1191,25 +1262,28 @@
         <v>100</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I4" t="s">
         <v>93</v>
       </c>
       <c r="J4" t="s">
-        <v>168</v>
-      </c>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="K4" t="s">
+        <v>206</v>
+      </c>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>23</v>
@@ -1224,25 +1298,25 @@
         <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="J5" t="s">
-        <v>96</v>
-      </c>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>26</v>
@@ -1257,31 +1331,34 @@
         <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
-      </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="K6" t="s">
+        <v>206</v>
+      </c>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E7">
         <v>6.1</v>
@@ -1290,31 +1367,31 @@
         <v>50</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H7" s="5">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="J7" t="s">
-        <v>96</v>
-      </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
       <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="E8">
         <v>6.7</v>
@@ -1323,31 +1400,31 @@
         <v>100</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I8" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="J8" t="s">
+        <v>209</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E9">
         <v>6.7</v>
@@ -1356,30 +1433,33 @@
         <v>50</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I9" t="s">
         <v>93</v>
       </c>
       <c r="J9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="K9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E10">
         <v>6.3</v>
@@ -1388,30 +1468,30 @@
         <v>150</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="J10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E11">
         <v>7.4</v>
@@ -1420,26 +1500,29 @@
         <v>150</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="J11" t="s">
-        <v>96</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I48 I50:I1048576" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I50:J1048576 I2:I48 J12:J48" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
       <formula1>Categories_Range</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8 G10:G48" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
       <formula1>"Low,High"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:L11 J2:J11" xr:uid="{80DF18E4-CD06-4E48-8072-6915464D3172}">
+      <formula1>Topics_Range</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1473,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A9A40E-25F0-458E-A251-DF2D64A47FEF}">
-  <dimension ref="A1:M77"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1488,10 +1571,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J1" t="s">
         <v>94</v>
@@ -1508,16 +1591,16 @@
         <v>6.3</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1531,10 +1614,10 @@
         <v>5.6</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1548,7 +1631,7 @@
         <v>6.8</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J4" t="s">
         <v>95</v>
@@ -1565,13 +1648,13 @@
         <v>6.4</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J5" t="s">
+        <v>151</v>
+      </c>
+      <c r="L5" t="s">
         <v>155</v>
-      </c>
-      <c r="L5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1585,13 +1668,13 @@
         <v>6.6</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="L6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1605,7 +1688,7 @@
         <v>6.5</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J7" t="s">
         <v>95</v>
@@ -1613,7 +1696,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>31</v>
@@ -1622,15 +1705,15 @@
         <v>7</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>32</v>
@@ -1639,13 +1722,13 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J9" t="s">
         <v>95</v>
       </c>
       <c r="L9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1659,13 +1742,13 @@
         <v>5.3</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J10" t="s">
         <v>95</v>
       </c>
       <c r="L10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1683,18 +1766,18 @@
         <v>6.4</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J12" t="s">
         <v>93</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>45</v>
@@ -1703,13 +1786,13 @@
         <v>6.2</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J13" t="s">
         <v>93</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1723,13 +1806,13 @@
         <v>6.6</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J14" t="s">
         <v>95</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1743,16 +1826,16 @@
         <v>6.3</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J15" t="s">
         <v>95</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="M15" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1766,13 +1849,16 @@
         <v>6.1</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J16" t="s">
         <v>95</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+      <c r="M16" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1786,13 +1872,13 @@
         <v>6.3</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J17" t="s">
         <v>95</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1806,7 +1892,7 @@
         <v>6.3</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J18" t="s">
         <v>95</v>
@@ -1824,13 +1910,13 @@
         <v>6.7</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J19" t="s">
         <v>95</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1844,13 +1930,13 @@
         <v>6</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J20" t="s">
         <v>95</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -1859,10 +1945,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H22">
         <v>6.8</v>
@@ -1871,7 +1957,7 @@
         <v>93</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1880,44 +1966,44 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H24">
         <v>6.8</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H25">
         <v>6.9</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J25" t="s">
         <v>95</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H26">
         <v>6.2</v>
@@ -1926,41 +2012,41 @@
         <v>95</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H27">
         <v>6.3</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J27" t="s">
         <v>95</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H28">
         <v>6.1</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J28" t="s">
         <v>95</v>
@@ -2098,18 +2184,18 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -2137,71 +2223,71 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -2214,47 +2300,103 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>193</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>194</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>196</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>198</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>203</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>214</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2321,9 +2463,16 @@
     <hyperlink ref="B28" r:id="rId52" xr:uid="{39D1A97D-1FE6-4AED-9283-406EA3C6F830}"/>
     <hyperlink ref="B75" r:id="rId53" xr:uid="{D501DC89-012E-4E1D-9617-AC01F33BF8D0}"/>
     <hyperlink ref="B77" r:id="rId54" xr:uid="{7DA3A161-A8F2-4139-8497-DAECF70018E5}"/>
+    <hyperlink ref="B78" r:id="rId55" xr:uid="{A306BE58-8655-4B3E-B065-CAB1F9C723D8}"/>
+    <hyperlink ref="B79" r:id="rId56" xr:uid="{E2C39033-2C18-486E-8BC9-8D4ACEEE5A8F}"/>
+    <hyperlink ref="B80" r:id="rId57" xr:uid="{46FC8386-EC0E-45F5-9DBB-3B56D5712661}"/>
+    <hyperlink ref="B81" r:id="rId58" xr:uid="{B9661603-9D9A-45E0-9498-F7B2379EDAC0}"/>
+    <hyperlink ref="B82" r:id="rId59" xr:uid="{DBA6B0B8-4717-4960-B067-E4D7903303FE}"/>
+    <hyperlink ref="B83" r:id="rId60" xr:uid="{5BCCEDE0-B87F-4733-81B6-549CF14AB475}"/>
+    <hyperlink ref="B84" r:id="rId61" xr:uid="{4080C57B-4807-4D4E-99FE-26EA71B76949}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId62"/>
 </worksheet>
 </file>
 
@@ -2332,7 +2481,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2352,17 +2501,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2376,12 +2525,56 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14353F15-E5ED-437F-B1CC-0C6B2FAC05B1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
readme update script fixed
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BEFD50-22F5-42C9-BBA1-CFE68318F8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFD7854-6C4E-47D8-98A4-AF9C39AE0E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -1124,7 +1124,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Gold Fever added Criss Cross (in progress)
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2B1223-69E6-4D3E-BE37-208E6129148A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DDF34E-143A-4403-B8F9-681208E4AEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="281">
   <si>
     <t>Pig</t>
   </si>
@@ -155,9 +155,6 @@
     <t>https://boardgamegeek.com/boardgame/220988/criss-cross</t>
   </si>
   <si>
-    <t>Criss cross</t>
-  </si>
-  <si>
     <t>https://boardgamegeek.com/boardgame/41493/yamslam</t>
   </si>
   <si>
@@ -434,9 +431,6 @@
     <t>https://boardgamegeek.com/boardgame/7476/complica</t>
   </si>
   <si>
-    <t>King's valley</t>
-  </si>
-  <si>
     <t>https://boardgamegeek.com/boardgame/86169/kings-valley</t>
   </si>
   <si>
@@ -831,6 +825,66 @@
   </si>
   <si>
     <t>kings-valley</t>
+  </si>
+  <si>
+    <t>King's Valley</t>
+  </si>
+  <si>
+    <t>https://www.ultraboardgames.com/quixo/game-rules.php</t>
+  </si>
+  <si>
+    <t>quixo</t>
+  </si>
+  <si>
+    <t>Breakthru</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/335/breakthru</t>
+  </si>
+  <si>
+    <t>Gyges</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/10527/gyges</t>
+  </si>
+  <si>
+    <t>Land 6</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/161849/land-6</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/40819/cheese-chasers</t>
+  </si>
+  <si>
+    <t>Cheese Chasers</t>
+  </si>
+  <si>
+    <t>Catchup</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/68199/catchup</t>
+  </si>
+  <si>
+    <t>Gold Fever</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/234120/gold-fever</t>
+  </si>
+  <si>
+    <t>SIMPLE but use without Ruby &amp; Emerald</t>
+  </si>
+  <si>
+    <t>Venice conn</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/1910/venice-connection</t>
+  </si>
+  <si>
+    <t>gold-fever</t>
+  </si>
+  <si>
+    <t>http://strongholdgames.com/our-games/gold-fever/</t>
   </si>
 </sst>
 </file>
@@ -926,8 +980,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K16" totalsRowShown="0">
-  <autoFilter ref="A1:K16" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K17" totalsRowShown="0">
+  <autoFilter ref="A1:K17" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A79D0D46-4EBF-4D48-8DFC-C1F9B9F5B13B}" name="Name"/>
     <tableColumn id="10" xr3:uid="{0B874210-D71E-4787-AC57-435630C4FB1F}" name="Folder"/>
@@ -1262,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA158D42-EF44-4D25-B732-21E60DAA7307}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1287,34 +1341,34 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1322,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1337,31 +1391,31 @@
         <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H2" s="5">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>5.9</v>
@@ -1370,31 +1424,31 @@
         <v>50</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="5">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4">
         <v>5.0999999999999996</v>
@@ -1403,34 +1457,34 @@
         <v>100</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" t="s">
+        <v>188</v>
+      </c>
+      <c r="K4" t="s">
         <v>190</v>
-      </c>
-      <c r="K4" t="s">
-        <v>192</v>
       </c>
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5">
         <v>6.1</v>
@@ -1439,31 +1493,31 @@
         <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6">
         <v>7.1</v>
@@ -1472,19 +1526,19 @@
         <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K6" t="s">
         <v>190</v>
-      </c>
-      <c r="K6" t="s">
-        <v>192</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -1493,13 +1547,13 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7">
         <v>6.1</v>
@@ -1508,34 +1562,34 @@
         <v>50</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" s="5">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E8">
         <v>6.7</v>
@@ -1544,34 +1598,34 @@
         <v>100</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="E9">
         <v>6.7</v>
@@ -1580,33 +1634,33 @@
         <v>50</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J9" t="s">
+        <v>188</v>
+      </c>
+      <c r="K9" t="s">
         <v>190</v>
-      </c>
-      <c r="K9" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="E10">
         <v>6.3</v>
@@ -1615,30 +1669,30 @@
         <v>150</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E11">
         <v>7.4</v>
@@ -1647,33 +1701,33 @@
         <v>150</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E12">
         <v>6.4</v>
@@ -1682,48 +1736,48 @@
         <v>100</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E13">
         <v>6.4</v>
       </c>
       <c r="F13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>91</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1731,13 +1785,13 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E14">
         <v>5.6</v>
@@ -1746,33 +1800,33 @@
         <v>25</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>261</v>
       </c>
       <c r="B15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E15">
         <v>6.5</v>
@@ -1784,36 +1838,86 @@
         <v>91</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="B16" t="s">
+        <v>263</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D16" s="1"/>
+        <v>224</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E16">
+        <v>6.2</v>
+      </c>
       <c r="F16" t="s">
-        <v>259</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
+        <v>257</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B17" t="s">
+        <v>279</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E17">
+        <v>6.4</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" t="s">
+        <v>151</v>
+      </c>
+      <c r="J17" t="s">
+        <v>189</v>
+      </c>
+      <c r="K17" t="s">
+        <v>188</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I16" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I17" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
       <formula1>Categories_Range</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8 G10:G12" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
@@ -1851,21 +1955,23 @@
     <hyperlink ref="C15" r:id="rId25" xr:uid="{91E3AA44-1161-40E0-A15C-324284007D73}"/>
     <hyperlink ref="C16" r:id="rId26" xr:uid="{E8B5F339-5B15-4F97-8B7D-4FB28F4DC07C}"/>
     <hyperlink ref="D15" r:id="rId27" xr:uid="{91790606-D10A-4BB9-A6BF-5EF617AA34EB}"/>
+    <hyperlink ref="D16" r:id="rId28" xr:uid="{C0B23ACB-FDAA-445C-9509-65684AC62983}"/>
+    <hyperlink ref="C17" r:id="rId29" xr:uid="{E7B3FDEC-5073-476A-80FE-8E262A277461}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId30"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A9A40E-25F0-458E-A251-DF2D64A47FEF}">
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1877,13 +1983,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1897,1010 +2003,1041 @@
         <v>6.3</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J2" t="s">
         <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>6.8</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H4">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>140</v>
       </c>
       <c r="J4" t="s">
-        <v>85</v>
+        <v>141</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>6.5</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H6">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J6" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>145</v>
+      <c r="M6" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H7">
-        <v>6.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="L7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="H8">
-        <v>7</v>
+        <v>5.3</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J8" t="s">
-        <v>147</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="M8" t="s">
-        <v>249</v>
+        <v>84</v>
+      </c>
+      <c r="L8" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="H9">
-        <v>4.9000000000000004</v>
+        <v>6.2</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J9" t="s">
-        <v>85</v>
-      </c>
-      <c r="L9" t="s">
-        <v>145</v>
+        <v>82</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H10">
-        <v>5.3</v>
+        <v>6.6</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
-      </c>
-      <c r="L10" t="s">
-        <v>145</v>
+        <v>84</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="L11" s="7"/>
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11">
+        <v>6.3</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J11" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="M11" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H12">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="J12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13">
-        <v>6.2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="J13" t="s">
-        <v>83</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>145</v>
+      <c r="B13" s="1"/>
+      <c r="L13" s="7"/>
+      <c r="M13" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H14">
-        <v>6.6</v>
+        <v>6.3</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>145</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="H15">
-        <v>6.3</v>
+        <v>6.7</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="M15" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="H16">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="L17" s="7"/>
-      <c r="M17" t="s">
-        <v>181</v>
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17">
+        <v>6.8</v>
+      </c>
+      <c r="J17" t="s">
+        <v>82</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>122</v>
       </c>
       <c r="H18">
-        <v>6.3</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="J18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L18" s="7"/>
+        <v>6.8</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="H19">
-        <v>6.7</v>
+        <v>6.9</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="H20">
-        <v>6</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>140</v>
+        <v>6.2</v>
       </c>
       <c r="J20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>156</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="H21">
-        <v>6.8</v>
+        <v>6.3</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="J21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="H22">
-        <v>6.8</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>145</v>
-      </c>
+        <v>6.1</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J22" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H23">
-        <v>6.9</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" t="s">
-        <v>85</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>149</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H24">
-        <v>6.2</v>
-      </c>
-      <c r="J24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>145</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H25">
-        <v>6.3</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J25" t="s">
-        <v>85</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>145</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>173</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H26">
-        <v>6.1</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="J26" t="s">
-        <v>85</v>
-      </c>
-      <c r="L26" s="7"/>
+        <v>31</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
+      </c>
+      <c r="J28" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="J32" t="s">
-        <v>85</v>
+        <v>193</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="M32" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>63</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J36" t="s">
-        <v>195</v>
-      </c>
-      <c r="L36" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="M36" t="s">
-        <v>260</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
+      </c>
+      <c r="J37" t="s">
+        <v>82</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="M37" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="J41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="M41" t="s">
-        <v>248</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J45" t="s">
-        <v>83</v>
-      </c>
-      <c r="L45" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>117</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J51" t="s">
+        <v>197</v>
+      </c>
+      <c r="K51" t="s">
+        <v>239</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>128</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J55" t="s">
-        <v>199</v>
-      </c>
-      <c r="K55" t="s">
-        <v>241</v>
-      </c>
-      <c r="L55" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>133</v>
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K58" t="s">
+        <v>240</v>
+      </c>
+      <c r="L58" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="M58" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>12</v>
+        <v>169</v>
+      </c>
+      <c r="K59" t="s">
+        <v>251</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>166</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="K62" t="s">
-        <v>242</v>
-      </c>
-      <c r="L62" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="M62" t="s">
-        <v>254</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="L62" s="7"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>170</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K63" t="s">
-        <v>253</v>
-      </c>
-      <c r="L63" s="7" t="s">
-        <v>145</v>
-      </c>
+      <c r="B63" s="1"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>177</v>
+        <v>182</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>178</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="K66" t="s">
-        <v>247</v>
-      </c>
-      <c r="L66" s="7"/>
+      <c r="B66" s="1"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B67" s="1"/>
+      <c r="A67" t="s">
+        <v>184</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K67" t="s">
+        <v>242</v>
+      </c>
+      <c r="L67" s="7" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
+      </c>
+      <c r="K68" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>184</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>185</v>
+      <c r="B69" s="1"/>
+      <c r="M69" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B70" s="1"/>
+      <c r="M70" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="K71" t="s">
         <v>244</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="M71" t="s">
+        <v>253</v>
+      </c>
+      <c r="N71" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="K72" t="s">
         <v>243</v>
       </c>
+      <c r="L72" s="7" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B73" s="1"/>
-      <c r="M73" t="s">
-        <v>257</v>
+      <c r="A73" t="s">
+        <v>206</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B74" s="1"/>
-      <c r="M74" t="s">
-        <v>258</v>
+      <c r="A74" t="s">
+        <v>211</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="K75" t="s">
-        <v>246</v>
-      </c>
-      <c r="L75" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="M75" t="s">
-        <v>255</v>
-      </c>
-      <c r="N75" t="s">
-        <v>256</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="L75" s="7"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K76" t="s">
-        <v>245</v>
-      </c>
-      <c r="L76" s="7" t="s">
-        <v>145</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>214</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="K78" t="s">
+        <v>250</v>
+      </c>
+      <c r="L78" s="7"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="K79" t="s">
-        <v>250</v>
-      </c>
-      <c r="L79" s="7"/>
+        <v>249</v>
+      </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>217</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L80" s="7"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>221</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="K82" t="s">
-        <v>252</v>
-      </c>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
       <c r="L82" s="7"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="K83" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L84" s="7"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>229</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B86" s="1"/>
-      <c r="L86" s="7"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>233</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>231</v>
+        <v>264</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>235</v>
+        <v>268</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>239</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>272</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L94" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="M94" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>277</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8E64C7A1-5801-4044-B589-D487C836BFCF}"/>
-    <hyperlink ref="B59" r:id="rId2" xr:uid="{7BEC1253-D118-4590-AF24-CDE738F8B1D8}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{9B7928A1-3A7E-46CC-AA5A-B57923DDFA32}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{1BC6A08D-1D08-4623-8C82-B71A0592AAB6}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{852CA370-9A08-4A1C-B844-C12255B3943D}"/>
-    <hyperlink ref="B8" r:id="rId6" xr:uid="{E666E340-63E8-4663-948F-406098389801}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{4C6A5B99-F01F-4E74-84FF-89478DB73084}"/>
-    <hyperlink ref="B28" r:id="rId8" xr:uid="{6F79CD7B-678A-4274-89B4-B9544BE83041}"/>
-    <hyperlink ref="B29" r:id="rId9" xr:uid="{9211F0DC-E5BA-4E37-8711-10B29744A713}"/>
-    <hyperlink ref="B30" r:id="rId10" xr:uid="{44B7F867-AC69-4A22-83B6-46E52511ACAE}"/>
-    <hyperlink ref="B31" r:id="rId11" xr:uid="{F4B22872-BE08-49A5-9D25-B40B43B58B00}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{D8FD9E36-7834-451C-BCEA-39AEBB29495C}"/>
-    <hyperlink ref="B13" r:id="rId13" xr:uid="{D415E350-C5ED-4B12-9A8A-72DFD905618E}"/>
-    <hyperlink ref="B32" r:id="rId14" xr:uid="{2DE0CFB5-2C9F-4FF0-AAD0-15FADBF567E0}"/>
-    <hyperlink ref="B14" r:id="rId15" xr:uid="{9CCFFBB9-3B72-4FB7-94F3-1C8439CA8D47}"/>
-    <hyperlink ref="B15" r:id="rId16" xr:uid="{5C9F6E2F-3112-48A6-B5B3-72043F9FA591}"/>
-    <hyperlink ref="B16" r:id="rId17" xr:uid="{DDFD90C3-8BF5-4CA2-96A4-256D35D2D59E}"/>
-    <hyperlink ref="B27" r:id="rId18" xr:uid="{7598335B-1BBA-46B0-B82C-77CC49C095EF}"/>
-    <hyperlink ref="B18" r:id="rId19" xr:uid="{D29184C3-5D1A-443B-9B34-4C4114F1E387}"/>
-    <hyperlink ref="B19" r:id="rId20" xr:uid="{DE020276-739E-4605-82CA-4152C2825027}"/>
-    <hyperlink ref="B34" r:id="rId21" xr:uid="{5A0FEA15-888C-4075-9C2F-CFD8546985A7}"/>
-    <hyperlink ref="B35" r:id="rId22" xr:uid="{2C05C520-6C02-4D0C-BB87-EEDF41E33FC8}"/>
-    <hyperlink ref="B36" r:id="rId23" xr:uid="{A827F7CF-12E3-44AE-BBD1-1A9A96F3FB02}"/>
-    <hyperlink ref="B37" r:id="rId24" xr:uid="{A1A4F6A6-F4E7-42AF-B52D-3A521F5406E5}"/>
-    <hyperlink ref="B20" r:id="rId25" xr:uid="{28FFB9B7-2753-4040-946E-FF2B9EA9EC0B}"/>
-    <hyperlink ref="B38" r:id="rId26" xr:uid="{FE39472A-D9C9-4EF0-AEBC-06F8FF1443E7}"/>
-    <hyperlink ref="B39" r:id="rId27" xr:uid="{1108D29F-FA18-4293-B305-A0EF22F38E43}"/>
-    <hyperlink ref="B42" r:id="rId28" xr:uid="{BD40941F-3476-49F4-A2FE-4355F43FFB72}"/>
-    <hyperlink ref="B43" r:id="rId29" xr:uid="{48489DD5-0C1A-4332-ADD5-32201C6C680E}"/>
-    <hyperlink ref="B44" r:id="rId30" xr:uid="{0E8C2D49-C640-4491-A333-E7657B4A3672}"/>
-    <hyperlink ref="B45" r:id="rId31" xr:uid="{75E85909-D109-431E-9850-DDF0148E901E}"/>
-    <hyperlink ref="B21" r:id="rId32" xr:uid="{5E39EF7D-055F-4DB2-BB3B-A0F841DB8313}"/>
-    <hyperlink ref="B47" r:id="rId33" xr:uid="{13E723D6-1FD1-4E3C-A566-3BBB021EE312}"/>
-    <hyperlink ref="B48" r:id="rId34" xr:uid="{26A32048-9EC8-4145-AB5D-8A9AB962E3BF}"/>
-    <hyperlink ref="B22" r:id="rId35" xr:uid="{20635745-E571-4992-9762-4A7AF1CE514E}"/>
-    <hyperlink ref="B52" r:id="rId36" xr:uid="{0245698D-0017-4BE5-BA95-484935FE4171}"/>
-    <hyperlink ref="B23" r:id="rId37" xr:uid="{F3942003-110E-425E-A163-21049FB9CB8F}"/>
-    <hyperlink ref="B54" r:id="rId38" xr:uid="{D2FED77C-07F4-432A-9101-560A5C83BEB5}"/>
-    <hyperlink ref="B56" r:id="rId39" xr:uid="{E5D8CB8A-64AD-48E3-A774-63A0FA6EA437}"/>
-    <hyperlink ref="B24" r:id="rId40" xr:uid="{7C42C010-5880-480F-AA12-C5D610003B9E}"/>
-    <hyperlink ref="B40" r:id="rId41" xr:uid="{5A6573CB-BC16-4292-801B-D3EC4C9D3130}"/>
-    <hyperlink ref="B41" r:id="rId42" xr:uid="{E6BEA243-9351-4DF7-B6D2-70D9924B0513}"/>
-    <hyperlink ref="B61" r:id="rId43" xr:uid="{1B239E16-A845-4BEF-A0FE-5AB8E59A9B80}"/>
-    <hyperlink ref="B62" r:id="rId44" xr:uid="{6E07CA5E-F80F-4621-B1F0-EC866F5962EA}"/>
-    <hyperlink ref="B63" r:id="rId45" xr:uid="{6398F33C-7815-4044-B5C2-C9C95DFB7F47}"/>
-    <hyperlink ref="B26" r:id="rId46" xr:uid="{39D1A97D-1FE6-4AED-9283-406EA3C6F830}"/>
-    <hyperlink ref="B64" r:id="rId47" xr:uid="{D501DC89-012E-4E1D-9617-AC01F33BF8D0}"/>
-    <hyperlink ref="B66" r:id="rId48" xr:uid="{7DA3A161-A8F2-4139-8497-DAECF70018E5}"/>
-    <hyperlink ref="B68" r:id="rId49" xr:uid="{E2C39033-2C18-486E-8BC9-8D4ACEEE5A8F}"/>
-    <hyperlink ref="B69" r:id="rId50" xr:uid="{46FC8386-EC0E-45F5-9DBB-3B56D5712661}"/>
-    <hyperlink ref="B71" r:id="rId51" xr:uid="{DBA6B0B8-4717-4960-B067-E4D7903303FE}"/>
-    <hyperlink ref="B72" r:id="rId52" xr:uid="{5BCCEDE0-B87F-4733-81B6-549CF14AB475}"/>
-    <hyperlink ref="B75" r:id="rId53" xr:uid="{4080C57B-4807-4D4E-99FE-26EA71B76949}"/>
-    <hyperlink ref="B76" r:id="rId54" xr:uid="{6234C51E-BA4E-4F25-92F0-8D4C68776565}"/>
-    <hyperlink ref="B77" r:id="rId55" xr:uid="{45E304E3-DF2C-4C31-9036-211FC61B6762}"/>
-    <hyperlink ref="B78" r:id="rId56" xr:uid="{59415891-A3CC-451F-8C8A-ECDC55774A98}"/>
-    <hyperlink ref="B79" r:id="rId57" xr:uid="{84DD642F-46B9-416B-B48E-94FCEED3BD21}"/>
-    <hyperlink ref="B80" r:id="rId58" xr:uid="{88C07BA3-40B3-4DB0-ADB6-EBCD37CDF728}"/>
-    <hyperlink ref="B81" r:id="rId59" xr:uid="{EB488184-7521-426C-8E5F-9D3F7143FABD}"/>
-    <hyperlink ref="B82" r:id="rId60" xr:uid="{C9DA6395-91D4-40FF-8703-94862162E322}"/>
-    <hyperlink ref="B83" r:id="rId61" xr:uid="{458AAD68-E139-46C5-8642-0DCEC22F6A18}"/>
-    <hyperlink ref="B85" r:id="rId62" xr:uid="{EA708719-68FD-4E7B-AA09-C6ED4AC0C8F5}"/>
-    <hyperlink ref="B87" r:id="rId63" xr:uid="{43682E17-B058-4CB3-88F9-E3F669C706B9}"/>
-    <hyperlink ref="B88" r:id="rId64" xr:uid="{680F58E4-3DCD-4646-9147-4890C367E5E4}"/>
-    <hyperlink ref="B89" r:id="rId65" xr:uid="{C4B8CBDB-748D-460C-957D-D7352D097E7C}"/>
-    <hyperlink ref="B90" r:id="rId66" xr:uid="{E3A3C38C-D0FA-4507-82C6-0F107988A9B5}"/>
-    <hyperlink ref="B91" r:id="rId67" xr:uid="{6D53A403-E1BE-4743-B349-E92F34D98F59}"/>
+    <hyperlink ref="B55" r:id="rId2" xr:uid="{7BEC1253-D118-4590-AF24-CDE738F8B1D8}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{9B7928A1-3A7E-46CC-AA5A-B57923DDFA32}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{1BC6A08D-1D08-4623-8C82-B71A0592AAB6}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{852CA370-9A08-4A1C-B844-C12255B3943D}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{E666E340-63E8-4663-948F-406098389801}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{4C6A5B99-F01F-4E74-84FF-89478DB73084}"/>
+    <hyperlink ref="B24" r:id="rId8" xr:uid="{6F79CD7B-678A-4274-89B4-B9544BE83041}"/>
+    <hyperlink ref="B25" r:id="rId9" xr:uid="{9211F0DC-E5BA-4E37-8711-10B29744A713}"/>
+    <hyperlink ref="B26" r:id="rId10" xr:uid="{44B7F867-AC69-4A22-83B6-46E52511ACAE}"/>
+    <hyperlink ref="B27" r:id="rId11" xr:uid="{F4B22872-BE08-49A5-9D25-B40B43B58B00}"/>
+    <hyperlink ref="B9" r:id="rId12" xr:uid="{D415E350-C5ED-4B12-9A8A-72DFD905618E}"/>
+    <hyperlink ref="B28" r:id="rId13" xr:uid="{2DE0CFB5-2C9F-4FF0-AAD0-15FADBF567E0}"/>
+    <hyperlink ref="B10" r:id="rId14" xr:uid="{9CCFFBB9-3B72-4FB7-94F3-1C8439CA8D47}"/>
+    <hyperlink ref="B11" r:id="rId15" xr:uid="{5C9F6E2F-3112-48A6-B5B3-72043F9FA591}"/>
+    <hyperlink ref="B12" r:id="rId16" xr:uid="{DDFD90C3-8BF5-4CA2-96A4-256D35D2D59E}"/>
+    <hyperlink ref="B23" r:id="rId17" xr:uid="{7598335B-1BBA-46B0-B82C-77CC49C095EF}"/>
+    <hyperlink ref="B14" r:id="rId18" xr:uid="{D29184C3-5D1A-443B-9B34-4C4114F1E387}"/>
+    <hyperlink ref="B15" r:id="rId19" xr:uid="{DE020276-739E-4605-82CA-4152C2825027}"/>
+    <hyperlink ref="B30" r:id="rId20" xr:uid="{5A0FEA15-888C-4075-9C2F-CFD8546985A7}"/>
+    <hyperlink ref="B31" r:id="rId21" xr:uid="{2C05C520-6C02-4D0C-BB87-EEDF41E33FC8}"/>
+    <hyperlink ref="B32" r:id="rId22" xr:uid="{A827F7CF-12E3-44AE-BBD1-1A9A96F3FB02}"/>
+    <hyperlink ref="B33" r:id="rId23" xr:uid="{A1A4F6A6-F4E7-42AF-B52D-3A521F5406E5}"/>
+    <hyperlink ref="B16" r:id="rId24" xr:uid="{28FFB9B7-2753-4040-946E-FF2B9EA9EC0B}"/>
+    <hyperlink ref="B34" r:id="rId25" xr:uid="{FE39472A-D9C9-4EF0-AEBC-06F8FF1443E7}"/>
+    <hyperlink ref="B35" r:id="rId26" xr:uid="{1108D29F-FA18-4293-B305-A0EF22F38E43}"/>
+    <hyperlink ref="B38" r:id="rId27" xr:uid="{BD40941F-3476-49F4-A2FE-4355F43FFB72}"/>
+    <hyperlink ref="B39" r:id="rId28" xr:uid="{48489DD5-0C1A-4332-ADD5-32201C6C680E}"/>
+    <hyperlink ref="B40" r:id="rId29" xr:uid="{0E8C2D49-C640-4491-A333-E7657B4A3672}"/>
+    <hyperlink ref="B41" r:id="rId30" xr:uid="{75E85909-D109-431E-9850-DDF0148E901E}"/>
+    <hyperlink ref="B17" r:id="rId31" xr:uid="{5E39EF7D-055F-4DB2-BB3B-A0F841DB8313}"/>
+    <hyperlink ref="B43" r:id="rId32" xr:uid="{13E723D6-1FD1-4E3C-A566-3BBB021EE312}"/>
+    <hyperlink ref="B44" r:id="rId33" xr:uid="{26A32048-9EC8-4145-AB5D-8A9AB962E3BF}"/>
+    <hyperlink ref="B18" r:id="rId34" xr:uid="{20635745-E571-4992-9762-4A7AF1CE514E}"/>
+    <hyperlink ref="B48" r:id="rId35" xr:uid="{0245698D-0017-4BE5-BA95-484935FE4171}"/>
+    <hyperlink ref="B19" r:id="rId36" xr:uid="{F3942003-110E-425E-A163-21049FB9CB8F}"/>
+    <hyperlink ref="B50" r:id="rId37" xr:uid="{D2FED77C-07F4-432A-9101-560A5C83BEB5}"/>
+    <hyperlink ref="B52" r:id="rId38" xr:uid="{E5D8CB8A-64AD-48E3-A774-63A0FA6EA437}"/>
+    <hyperlink ref="B20" r:id="rId39" xr:uid="{7C42C010-5880-480F-AA12-C5D610003B9E}"/>
+    <hyperlink ref="B36" r:id="rId40" xr:uid="{5A6573CB-BC16-4292-801B-D3EC4C9D3130}"/>
+    <hyperlink ref="B37" r:id="rId41" xr:uid="{E6BEA243-9351-4DF7-B6D2-70D9924B0513}"/>
+    <hyperlink ref="B57" r:id="rId42" xr:uid="{1B239E16-A845-4BEF-A0FE-5AB8E59A9B80}"/>
+    <hyperlink ref="B58" r:id="rId43" xr:uid="{6E07CA5E-F80F-4621-B1F0-EC866F5962EA}"/>
+    <hyperlink ref="B59" r:id="rId44" xr:uid="{6398F33C-7815-4044-B5C2-C9C95DFB7F47}"/>
+    <hyperlink ref="B22" r:id="rId45" xr:uid="{39D1A97D-1FE6-4AED-9283-406EA3C6F830}"/>
+    <hyperlink ref="B60" r:id="rId46" xr:uid="{D501DC89-012E-4E1D-9617-AC01F33BF8D0}"/>
+    <hyperlink ref="B62" r:id="rId47" xr:uid="{7DA3A161-A8F2-4139-8497-DAECF70018E5}"/>
+    <hyperlink ref="B64" r:id="rId48" xr:uid="{E2C39033-2C18-486E-8BC9-8D4ACEEE5A8F}"/>
+    <hyperlink ref="B65" r:id="rId49" xr:uid="{46FC8386-EC0E-45F5-9DBB-3B56D5712661}"/>
+    <hyperlink ref="B67" r:id="rId50" xr:uid="{DBA6B0B8-4717-4960-B067-E4D7903303FE}"/>
+    <hyperlink ref="B68" r:id="rId51" xr:uid="{5BCCEDE0-B87F-4733-81B6-549CF14AB475}"/>
+    <hyperlink ref="B71" r:id="rId52" xr:uid="{4080C57B-4807-4D4E-99FE-26EA71B76949}"/>
+    <hyperlink ref="B72" r:id="rId53" xr:uid="{6234C51E-BA4E-4F25-92F0-8D4C68776565}"/>
+    <hyperlink ref="B73" r:id="rId54" xr:uid="{45E304E3-DF2C-4C31-9036-211FC61B6762}"/>
+    <hyperlink ref="B74" r:id="rId55" xr:uid="{59415891-A3CC-451F-8C8A-ECDC55774A98}"/>
+    <hyperlink ref="B75" r:id="rId56" xr:uid="{84DD642F-46B9-416B-B48E-94FCEED3BD21}"/>
+    <hyperlink ref="B76" r:id="rId57" xr:uid="{88C07BA3-40B3-4DB0-ADB6-EBCD37CDF728}"/>
+    <hyperlink ref="B77" r:id="rId58" xr:uid="{EB488184-7521-426C-8E5F-9D3F7143FABD}"/>
+    <hyperlink ref="B78" r:id="rId59" xr:uid="{C9DA6395-91D4-40FF-8703-94862162E322}"/>
+    <hyperlink ref="B79" r:id="rId60" xr:uid="{458AAD68-E139-46C5-8642-0DCEC22F6A18}"/>
+    <hyperlink ref="B81" r:id="rId61" xr:uid="{EA708719-68FD-4E7B-AA09-C6ED4AC0C8F5}"/>
+    <hyperlink ref="B83" r:id="rId62" xr:uid="{43682E17-B058-4CB3-88F9-E3F669C706B9}"/>
+    <hyperlink ref="B84" r:id="rId63" xr:uid="{680F58E4-3DCD-4646-9147-4890C367E5E4}"/>
+    <hyperlink ref="B85" r:id="rId64" xr:uid="{C4B8CBDB-748D-460C-957D-D7352D097E7C}"/>
+    <hyperlink ref="B86" r:id="rId65" xr:uid="{E3A3C38C-D0FA-4507-82C6-0F107988A9B5}"/>
+    <hyperlink ref="B87" r:id="rId66" xr:uid="{6D53A403-E1BE-4743-B349-E92F34D98F59}"/>
+    <hyperlink ref="B88" r:id="rId67" xr:uid="{39EFBC6D-7C8B-4350-AF34-681C92DD5E23}"/>
+    <hyperlink ref="B89" r:id="rId68" xr:uid="{6A40045C-8E0C-42DA-855C-9040C2E90809}"/>
+    <hyperlink ref="B90" r:id="rId69" xr:uid="{93E0EBFA-AEE1-459B-B3C3-E2E29D0BC88F}"/>
+    <hyperlink ref="B91" r:id="rId70" xr:uid="{A769A1D1-C3AB-4E05-8448-8D7663B2EEDA}"/>
+    <hyperlink ref="B92" r:id="rId71" xr:uid="{0CECCD05-407F-4B24-AF2E-01F25D4DBCBB}"/>
+    <hyperlink ref="B95" r:id="rId72" xr:uid="{68E07E2C-26A7-485C-932F-BA6D7C9A6ED7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId68"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId73"/>
 </worksheet>
 </file>
 
@@ -2919,32 +3056,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2971,37 +3108,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separate GOLO basic and GOLO Scorecard
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3371BC2-4B95-4A28-813A-F47D023E4F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC1814D-E338-4BA9-B3E7-3E3DA43C6D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="324">
   <si>
     <t>Pig</t>
   </si>
@@ -998,16 +998,22 @@
     <t>https://boardgamegeek.com/boardgame/9319/train-game</t>
   </si>
   <si>
-    <t>GOLO</t>
-  </si>
-  <si>
-    <t>golo</t>
-  </si>
-  <si>
     <t>https://www.zobmondo.com/products/golo-golf-dice-game</t>
   </si>
   <si>
     <t>1+</t>
+  </si>
+  <si>
+    <t>golo-scard</t>
+  </si>
+  <si>
+    <t>GOLO (scorecard)</t>
+  </si>
+  <si>
+    <t>GOLO (basic)</t>
+  </si>
+  <si>
+    <t>golo-basic</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1109,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K18" totalsRowShown="0">
-  <autoFilter ref="A1:K18" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K19" totalsRowShown="0">
+  <autoFilter ref="A1:K19" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A79D0D46-4EBF-4D48-8DFC-C1F9B9F5B13B}" name="Name"/>
     <tableColumn id="10" xr3:uid="{0B874210-D71E-4787-AC57-435630C4FB1F}" name="Folder"/>
@@ -1439,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA158D42-EF44-4D25-B732-21E60DAA7307}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2039,16 +2045,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B18" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>304</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E18">
         <v>5.6</v>
@@ -2060,7 +2066,7 @@
         <v>90</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I18" t="s">
         <v>82</v>
@@ -2069,13 +2075,48 @@
         <v>189</v>
       </c>
       <c r="K18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>321</v>
+      </c>
+      <c r="B19" t="s">
+        <v>320</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E19">
+        <v>5.6</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="I19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" t="s">
+        <v>189</v>
+      </c>
+      <c r="K19" t="s">
         <v>188</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I18" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I19" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
       <formula1>Categories_Range</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8 G10:G12" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
@@ -2128,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A9A40E-25F0-458E-A251-DF2D64A47FEF}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ship, Captain, & Crew
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5E10F4-BC8E-4661-AFF4-083F58E908BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA12269-4C97-4B02-9BD1-A8D578C91F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="341">
   <si>
     <t>Pig</t>
   </si>
@@ -1056,6 +1056,15 @@
   </si>
   <si>
     <t>https://boardgamegeek.com/boardgame/18812/ship-captain-and-crew</t>
+  </si>
+  <si>
+    <t>scc</t>
+  </si>
+  <si>
+    <t>Ship, Captain, &amp; Crew</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Ship,_captain,_and_crew</t>
   </si>
 </sst>
 </file>
@@ -1151,8 +1160,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K20" totalsRowShown="0">
-  <autoFilter ref="A1:K20" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K22" totalsRowShown="0">
+  <autoFilter ref="A1:K22" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A79D0D46-4EBF-4D48-8DFC-C1F9B9F5B13B}" name="Name"/>
     <tableColumn id="10" xr3:uid="{0B874210-D71E-4787-AC57-435630C4FB1F}" name="Folder"/>
@@ -1487,15 +1496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA158D42-EF44-4D25-B732-21E60DAA7307}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
@@ -2156,15 +2165,62 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5"/>
+      <c r="A20" t="s">
+        <v>339</v>
+      </c>
+      <c r="B20" t="s">
+        <v>338</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20" t="s">
+        <v>188</v>
+      </c>
+      <c r="K20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I20" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I22" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
       <formula1>Categories_Range</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8 G10:G12" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
@@ -2217,8 +2273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A9A40E-25F0-458E-A251-DF2D64A47FEF}">
   <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
blokus update (scoring) & bugfixes
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631C030A-2F72-4299-A22E-8C02236163A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD9561-965C-4F68-9C3A-BB5318E27BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -1508,7 +1508,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2225,7 +2225,7 @@
         <v>6.8</v>
       </c>
       <c r="F21">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
criss cross update + cli + tests
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD9561-965C-4F68-9C3A-BB5318E27BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C6E8BE-7E57-4361-8C85-BD33BDF37D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="344">
   <si>
     <t>Pig</t>
   </si>
@@ -1508,7 +1508,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1956,8 +1956,8 @@
       <c r="E13">
         <v>6.4</v>
       </c>
-      <c r="F13" t="s">
-        <v>257</v>
+      <c r="F13">
+        <v>100</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>91</v>
@@ -1967,6 +1967,12 @@
       </c>
       <c r="I13" t="s">
         <v>82</v>
+      </c>
+      <c r="J13" t="s">
+        <v>192</v>
+      </c>
+      <c r="K13" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
index update push-fight (in progress)
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C6E8BE-7E57-4361-8C85-BD33BDF37D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2521C4D4-A142-4634-B07C-4CD9209FAD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="346">
   <si>
     <t>Pig</t>
   </si>
@@ -1074,6 +1074,12 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Blokus</t>
+  </si>
+  <si>
+    <t>https://pushfightgame.com</t>
+  </si>
+  <si>
+    <t>push-fight</t>
   </si>
 </sst>
 </file>
@@ -1169,8 +1175,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K23" totalsRowShown="0">
-  <autoFilter ref="A1:K23" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}" name="Table2" displayName="Table2" ref="A1:K22" totalsRowShown="0">
+  <autoFilter ref="A1:K22" xr:uid="{74F4E283-56FB-4114-A991-9FFC0E72842C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K22">
+    <sortCondition ref="F1:F22"/>
+  </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A79D0D46-4EBF-4D48-8DFC-C1F9B9F5B13B}" name="Name"/>
     <tableColumn id="10" xr3:uid="{0B874210-D71E-4787-AC57-435630C4FB1F}" name="Folder"/>
@@ -1505,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA158D42-EF44-4D25-B732-21E60DAA7307}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1525,7 +1534,7 @@
     <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1560,7 +1569,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1592,97 +1601,136 @@
         <v>189</v>
       </c>
       <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="str">
+        <f>MID(C2,LEN("https://boardgamegeek.com/boardgame/ "),100)</f>
+        <v>161130/pig</v>
+      </c>
+      <c r="O2" t="str">
+        <f>MID(N2,1,FIND("/",N2)-1)</f>
+        <v>161130</v>
+      </c>
+      <c r="P2" t="str">
+        <f>J2&amp;IF(K2&lt;&gt;"",", "&amp;K2,"")</f>
+        <v>Basics</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>235</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>76</v>
+        <v>236</v>
       </c>
       <c r="E3">
-        <v>5.9</v>
+        <v>5.6</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="5">
-        <v>2</v>
+      <c r="H3" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="I3" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
       <c r="J3" t="s">
+        <v>189</v>
+      </c>
+      <c r="K3" t="s">
         <v>188</v>
       </c>
       <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N22" si="0">MID(C3,LEN("https://boardgamegeek.com/boardgame/ "),100)</f>
+        <v>2392/mastermind</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O22" si="1">MID(N3,1,FIND("/",N3)-1)</f>
+        <v>2392</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P22" si="2">J3&amp;IF(K3&lt;&gt;"",", "&amp;K3,"")</f>
+        <v>Basics, Arrays</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>322</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>323</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>304</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>77</v>
+        <v>318</v>
       </c>
       <c r="E4">
-        <v>5.0999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>90</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>100</v>
+        <v>319</v>
       </c>
       <c r="I4" t="s">
         <v>82</v>
       </c>
       <c r="J4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" t="s">
         <v>188</v>
       </c>
-      <c r="K4" t="s">
-        <v>190</v>
-      </c>
       <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>7270/golo</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="1"/>
+        <v>7270</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="2"/>
+        <v>Basics, Arrays</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="F5">
         <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
@@ -1691,119 +1739,164 @@
         <v>197</v>
       </c>
       <c r="J5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" t="str">
+        <f t="shared" si="0"/>
+        <v>2448/kalah</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="1"/>
+        <v>2448</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="2"/>
+        <v>Arrays</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6">
-        <v>7.1</v>
+        <v>6.1</v>
       </c>
       <c r="F6">
         <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>107</v>
+        <v>91</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="J6" t="s">
-        <v>188</v>
-      </c>
-      <c r="K6" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>7450/stop-gate</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="1"/>
+        <v>7450</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="2"/>
+        <v>2D Arrays</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E7">
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
       <c r="F7">
         <v>50</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="5">
-        <v>2</v>
+        <v>90</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="I7" t="s">
-        <v>197</v>
+        <v>151</v>
       </c>
       <c r="J7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>12942/no-thanks</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="1"/>
+        <v>12942</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="2"/>
+        <v>Arrays, Algorithms</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E8">
-        <v>6.7</v>
+        <v>6.1</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>106</v>
+      <c r="H8" s="5">
+        <v>2</v>
       </c>
       <c r="I8" t="s">
         <v>197</v>
       </c>
       <c r="J8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K8" t="s">
         <v>191</v>
       </c>
       <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>2389/othello</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="1"/>
+        <v>2389</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="2"/>
+        <v>2D Arrays, Algorithms+</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -1837,401 +1930,551 @@
       <c r="K9" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>246228/impact-battle-elements</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="1"/>
+        <v>246228</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="2"/>
+        <v>Arrays, Algorithms</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>274</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>278</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>120</v>
+        <v>275</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>160</v>
+        <v>279</v>
       </c>
       <c r="E10">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="F10">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>90</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="J10" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>188</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>234120/gold-fever</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="1"/>
+        <v>234120</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="2"/>
+        <v>Basics, Arrays</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>321</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>98</v>
+        <v>304</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>162</v>
+        <v>318</v>
       </c>
       <c r="E11">
-        <v>7.4</v>
+        <v>5.6</v>
       </c>
       <c r="F11">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>136</v>
+        <v>319</v>
       </c>
       <c r="I11" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="J11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="0"/>
+        <v>7270/golo</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="1"/>
+        <v>7270</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="2"/>
+        <v>Arrays, Algorithms</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>340</v>
       </c>
       <c r="B12" t="s">
-        <v>201</v>
+        <v>338</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>337</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>202</v>
+        <v>339</v>
       </c>
       <c r="E12">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>90</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>203</v>
+        <v>100</v>
       </c>
       <c r="I12" t="s">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="J12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>18812/ship-captain-and-crew</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="1"/>
+        <v>18812</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>Arrays, Algorithms</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>96</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>210</v>
+        <v>77</v>
       </c>
       <c r="E13">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F13">
         <v>100</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="I13" t="s">
         <v>82</v>
       </c>
       <c r="J13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K13" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>10502/poker-dice</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="1"/>
+        <v>10502</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="2"/>
+        <v>Arrays, Algorithms</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>235</v>
+        <v>104</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>236</v>
+        <v>108</v>
       </c>
       <c r="E14">
-        <v>5.6</v>
+        <v>6.7</v>
       </c>
       <c r="F14">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>203</v>
+        <v>91</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="I14" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="J14" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="K14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="0"/>
+        <v>101463/paletto</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="1"/>
+        <v>101463</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="2"/>
+        <v>Graphs, Algorithms+</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>261</v>
+        <v>200</v>
       </c>
       <c r="B15" t="s">
-        <v>260</v>
+        <v>201</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>259</v>
+        <v>202</v>
       </c>
       <c r="E15">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="F15">
         <v>100</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>138</v>
+        <v>203</v>
       </c>
       <c r="I15" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
       <c r="J15" t="s">
         <v>192</v>
       </c>
       <c r="K15" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>165/black-box</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="1"/>
+        <v>165</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="2"/>
+        <v>2D Arrays, Algorithms+</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B16" t="s">
-        <v>263</v>
+        <v>209</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>224</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="E16">
-        <v>6.2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>257</v>
+        <v>6.4</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>91</v>
       </c>
       <c r="H16" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" t="s">
+        <v>192</v>
+      </c>
+      <c r="K16" t="s">
+        <v>190</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>220988/criss-cross</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="1"/>
+        <v>220988</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="2"/>
+        <v>2D Arrays, Algorithms</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>261</v>
+      </c>
+      <c r="B17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E17">
+        <v>6.5</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>274</v>
-      </c>
-      <c r="B17" t="s">
-        <v>278</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E17">
-        <v>6.4</v>
-      </c>
-      <c r="F17">
-        <v>50</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="I17" t="s">
-        <v>151</v>
-      </c>
       <c r="J17" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="K17" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="0"/>
+        <v>86169/kings-valley</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="1"/>
+        <v>86169</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="2"/>
+        <v>2D Arrays, Algorithms</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>322</v>
+        <v>158</v>
       </c>
       <c r="B18" t="s">
-        <v>323</v>
+        <v>159</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>304</v>
+        <v>120</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>318</v>
+        <v>160</v>
       </c>
       <c r="E18">
-        <v>5.6</v>
+        <v>6.3</v>
       </c>
       <c r="F18">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>90</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>319</v>
+        <v>138</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>170</v>
       </c>
       <c r="J18" t="s">
         <v>189</v>
       </c>
-      <c r="K18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N18" t="str">
+        <f t="shared" si="0"/>
+        <v>201028/farmers-finances</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="1"/>
+        <v>201028</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="2"/>
+        <v>Basics</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>321</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>320</v>
+        <v>161</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>304</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>318</v>
+        <v>162</v>
       </c>
       <c r="E19">
-        <v>5.6</v>
+        <v>7.4</v>
       </c>
       <c r="F19">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>319</v>
+        <v>136</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
       <c r="J19" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="K19" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="0"/>
+        <v>245487/orchard-9-card-solitaire-game</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="1"/>
+        <v>245487</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="2"/>
+        <v>2D Arrays, Algorithms+</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B20" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>337</v>
+        <v>14</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="E20">
-        <v>5.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="F20">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>197</v>
       </c>
       <c r="J20" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="K20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="0"/>
+        <v>16395/blokus-duo</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="1"/>
+        <v>16395</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="2"/>
+        <v>2D Arrays, Algorithms+</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>341</v>
+        <v>223</v>
       </c>
       <c r="B21" t="s">
-        <v>342</v>
+        <v>263</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>224</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>343</v>
+        <v>262</v>
       </c>
       <c r="E21">
-        <v>6.8</v>
-      </c>
-      <c r="F21">
-        <v>200</v>
+        <v>6.2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>257</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>91</v>
@@ -2242,80 +2485,116 @@
       <c r="I21" t="s">
         <v>197</v>
       </c>
-      <c r="J21" t="s">
+      <c r="N21" t="str">
+        <f t="shared" si="0"/>
+        <v>3190/quixo</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="1"/>
+        <v>3190</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>296</v>
+      </c>
+      <c r="B22" t="s">
+        <v>345</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E22">
+        <v>7.4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>257</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J22" t="s">
         <v>192</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K22" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="5"/>
+      <c r="N22" t="str">
+        <f t="shared" si="0"/>
+        <v>54221/push-fight</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="1"/>
+        <v>54221</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="2"/>
+        <v>2D Arrays, Algorithms+</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I23" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
-      <formula1>Categories_Range</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8 G10:G12" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
       <formula1>"Low,High"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:L11 J12:K14" xr:uid="{80DF18E4-CD06-4E48-8072-6915464D3172}">
       <formula1>Topics_Range</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I22" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
+      <formula1>Categories_Range</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{CF91A9A8-16D3-46A3-B4B1-49E61D0DA972}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{8F09DA75-066C-43FA-8D05-CA97F600C29F}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{0E6F462A-3EC9-43B4-9F5E-A8E6181E37D5}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{B37EBDC9-F50E-4086-8DD1-F1506CC45A94}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{7E6DB0B1-E2CC-4783-A64C-DB82F8331083}"/>
-    <hyperlink ref="C3" r:id="rId6" xr:uid="{6D9E49B1-389C-43CE-9B9A-40B327F12E17}"/>
-    <hyperlink ref="D3" r:id="rId7" xr:uid="{A70581CF-E6D2-41F5-923B-5012984D7F6E}"/>
-    <hyperlink ref="D4" r:id="rId8" xr:uid="{144FF911-1729-4A7D-A726-F90BAF1814D9}"/>
-    <hyperlink ref="D5" r:id="rId9" xr:uid="{9AA8F919-944A-4208-82A9-3EF318CB21E1}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{92CAD6FF-E7FB-4128-86FB-2F7BA0A06735}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{D6CE8703-8F93-4882-BEFD-866FA986BE7E}"/>
-    <hyperlink ref="C8" r:id="rId12" xr:uid="{9CCF4779-4997-4826-B069-ED6AF8CD3D91}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{31A51631-0C88-4ABC-87FE-D5DBD5DA9A3D}"/>
+    <hyperlink ref="C13" r:id="rId3" xr:uid="{0E6F462A-3EC9-43B4-9F5E-A8E6181E37D5}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{B37EBDC9-F50E-4086-8DD1-F1506CC45A94}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{7E6DB0B1-E2CC-4783-A64C-DB82F8331083}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{6D9E49B1-389C-43CE-9B9A-40B327F12E17}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{A70581CF-E6D2-41F5-923B-5012984D7F6E}"/>
+    <hyperlink ref="D13" r:id="rId8" xr:uid="{144FF911-1729-4A7D-A726-F90BAF1814D9}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{9AA8F919-944A-4208-82A9-3EF318CB21E1}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{92CAD6FF-E7FB-4128-86FB-2F7BA0A06735}"/>
+    <hyperlink ref="D8" r:id="rId11" xr:uid="{D6CE8703-8F93-4882-BEFD-866FA986BE7E}"/>
+    <hyperlink ref="C14" r:id="rId12" xr:uid="{9CCF4779-4997-4826-B069-ED6AF8CD3D91}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{31A51631-0C88-4ABC-87FE-D5DBD5DA9A3D}"/>
     <hyperlink ref="C9" r:id="rId14" xr:uid="{E751E88E-5FF3-4FFC-A298-C92A80243714}"/>
-    <hyperlink ref="C10" r:id="rId15" xr:uid="{776CBF58-DDF1-4EF3-8413-F4CA801CDCC7}"/>
-    <hyperlink ref="D10" r:id="rId16" xr:uid="{513AA72A-9CF0-4130-AF38-4E77D16460D1}"/>
-    <hyperlink ref="D11" r:id="rId17" xr:uid="{E327BEBE-F953-42C1-8769-F8E5CD69EB9C}"/>
-    <hyperlink ref="C11" r:id="rId18" xr:uid="{C02C3B6A-9987-4C26-9285-2B118139009F}"/>
-    <hyperlink ref="D6" r:id="rId19" xr:uid="{BE718736-4E6D-47AC-9AF1-9A2048A1D488}"/>
-    <hyperlink ref="C12" r:id="rId20" xr:uid="{2C899C78-28A5-4F49-A004-87C60CD18A61}"/>
-    <hyperlink ref="D12" r:id="rId21" xr:uid="{14F31107-86EB-4EFD-88F7-62E722CBCB5A}"/>
-    <hyperlink ref="D13" r:id="rId22" xr:uid="{EECFD8BA-ED23-418F-AF5C-7B91C3FF2281}"/>
-    <hyperlink ref="C14" r:id="rId23" xr:uid="{E22397AE-E4B2-4D22-A621-CA9C7EE0873D}"/>
-    <hyperlink ref="D14" r:id="rId24" xr:uid="{F72D111F-DC9F-4204-B339-3C2892C37544}"/>
-    <hyperlink ref="C15" r:id="rId25" xr:uid="{91E3AA44-1161-40E0-A15C-324284007D73}"/>
-    <hyperlink ref="C16" r:id="rId26" xr:uid="{E8B5F339-5B15-4F97-8B7D-4FB28F4DC07C}"/>
-    <hyperlink ref="D15" r:id="rId27" xr:uid="{91790606-D10A-4BB9-A6BF-5EF617AA34EB}"/>
-    <hyperlink ref="D16" r:id="rId28" xr:uid="{C0B23ACB-FDAA-445C-9509-65684AC62983}"/>
-    <hyperlink ref="C17" r:id="rId29" xr:uid="{E7B3FDEC-5073-476A-80FE-8E262A277461}"/>
-    <hyperlink ref="C21" r:id="rId30" xr:uid="{299C6B7A-AACC-402C-B4F6-966C25D424A0}"/>
+    <hyperlink ref="C18" r:id="rId15" xr:uid="{776CBF58-DDF1-4EF3-8413-F4CA801CDCC7}"/>
+    <hyperlink ref="D18" r:id="rId16" xr:uid="{513AA72A-9CF0-4130-AF38-4E77D16460D1}"/>
+    <hyperlink ref="D19" r:id="rId17" xr:uid="{E327BEBE-F953-42C1-8769-F8E5CD69EB9C}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{C02C3B6A-9987-4C26-9285-2B118139009F}"/>
+    <hyperlink ref="D7" r:id="rId19" xr:uid="{BE718736-4E6D-47AC-9AF1-9A2048A1D488}"/>
+    <hyperlink ref="C15" r:id="rId20" xr:uid="{2C899C78-28A5-4F49-A004-87C60CD18A61}"/>
+    <hyperlink ref="D15" r:id="rId21" xr:uid="{14F31107-86EB-4EFD-88F7-62E722CBCB5A}"/>
+    <hyperlink ref="D16" r:id="rId22" xr:uid="{EECFD8BA-ED23-418F-AF5C-7B91C3FF2281}"/>
+    <hyperlink ref="C3" r:id="rId23" xr:uid="{E22397AE-E4B2-4D22-A621-CA9C7EE0873D}"/>
+    <hyperlink ref="D3" r:id="rId24" xr:uid="{F72D111F-DC9F-4204-B339-3C2892C37544}"/>
+    <hyperlink ref="C17" r:id="rId25" xr:uid="{91E3AA44-1161-40E0-A15C-324284007D73}"/>
+    <hyperlink ref="C21" r:id="rId26" xr:uid="{E8B5F339-5B15-4F97-8B7D-4FB28F4DC07C}"/>
+    <hyperlink ref="D17" r:id="rId27" xr:uid="{91790606-D10A-4BB9-A6BF-5EF617AA34EB}"/>
+    <hyperlink ref="D21" r:id="rId28" xr:uid="{C0B23ACB-FDAA-445C-9509-65684AC62983}"/>
+    <hyperlink ref="C10" r:id="rId29" xr:uid="{E7B3FDEC-5073-476A-80FE-8E262A277461}"/>
+    <hyperlink ref="C20" r:id="rId30" xr:uid="{299C6B7A-AACC-402C-B4F6-966C25D424A0}"/>
+    <hyperlink ref="C22" r:id="rId31" xr:uid="{ED0D3C45-6012-4A86-A382-1CA92AAAC3A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId32"/>
   <tableParts count="1">
-    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2325,7 +2604,7 @@
   <dimension ref="A1:N120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3369,15 +3648,7 @@
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>296</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="J99" t="s">
-        <v>197</v>
-      </c>
+      <c r="B99" s="1"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
@@ -3607,17 +3878,16 @@
     <hyperlink ref="B105" r:id="rId81" xr:uid="{AC9B10DC-D9A9-454B-9D9E-3FD1F8A07319}"/>
     <hyperlink ref="B106" r:id="rId82" xr:uid="{5D022F17-F884-404E-A982-9719A1F8B494}"/>
     <hyperlink ref="B107" r:id="rId83" xr:uid="{4482DC95-EFB4-4407-94EF-DE8D4C7C0F7E}"/>
-    <hyperlink ref="B99" r:id="rId84" xr:uid="{6C624B3C-8128-471C-A80A-9099B64F96B4}"/>
-    <hyperlink ref="B113" r:id="rId85" xr:uid="{320C8057-1444-4203-AD09-BE1724791689}"/>
-    <hyperlink ref="B114" r:id="rId86" xr:uid="{9D3F3235-411C-4B5B-BBEA-D1C1FAF2CF81}"/>
-    <hyperlink ref="C116" r:id="rId87" xr:uid="{132C82DC-A581-466D-9507-B56567CB6A71}"/>
-    <hyperlink ref="B117" r:id="rId88" xr:uid="{644F4562-5FCE-414F-9878-C40784FA3BC1}"/>
-    <hyperlink ref="B118" r:id="rId89" xr:uid="{442A4D2F-9280-4BAC-885F-E9BE7144D25E}"/>
-    <hyperlink ref="B119" r:id="rId90" xr:uid="{5067CC59-E44B-4C73-BEEB-A95B546DAE67}"/>
-    <hyperlink ref="B120" r:id="rId91" xr:uid="{DDADA373-94A9-4F9B-8409-6821EBDD568E}"/>
+    <hyperlink ref="B113" r:id="rId84" xr:uid="{320C8057-1444-4203-AD09-BE1724791689}"/>
+    <hyperlink ref="B114" r:id="rId85" xr:uid="{9D3F3235-411C-4B5B-BBEA-D1C1FAF2CF81}"/>
+    <hyperlink ref="C116" r:id="rId86" xr:uid="{132C82DC-A581-466D-9507-B56567CB6A71}"/>
+    <hyperlink ref="B117" r:id="rId87" xr:uid="{644F4562-5FCE-414F-9878-C40784FA3BC1}"/>
+    <hyperlink ref="B118" r:id="rId88" xr:uid="{442A4D2F-9280-4BAC-885F-E9BE7144D25E}"/>
+    <hyperlink ref="B119" r:id="rId89" xr:uid="{5067CC59-E44B-4C73-BEEB-A95B546DAE67}"/>
+    <hyperlink ref="B120" r:id="rId90" xr:uid="{DDADA373-94A9-4F9B-8409-6821EBDD568E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId92"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId91"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Push Fight: cli and tests
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Hg\board-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D351B8-BBEC-4849-8DA6-40FDF5D549D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3A1A26-1721-4C06-8547-32492CC2D3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E2C030E-03C5-45B9-A52C-AE882ABDD6B8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="405">
   <si>
     <t>Pig</t>
   </si>
@@ -1092,6 +1092,171 @@
   </si>
   <si>
     <t>https://boardgamegeek.com/boardgame/29952/quinamid</t>
+  </si>
+  <si>
+    <t>Diam</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/11730/diam</t>
+  </si>
+  <si>
+    <t>Double Shutter</t>
+  </si>
+  <si>
+    <t>Pikemen</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/20269/pikemen</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/34943/double-shutter</t>
+  </si>
+  <si>
+    <t>Cosmic Coasters</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/1771/cosmic-coasters</t>
+  </si>
+  <si>
+    <t>Kamon</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/28738/kamon</t>
+  </si>
+  <si>
+    <t>Qwixx Card</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/151835/qwixx-card-game</t>
+  </si>
+  <si>
+    <t>Ominoes</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/195484/ominoes</t>
+  </si>
+  <si>
+    <t>Fight!</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/2284/fight</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>Knight moves</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/21479/knight-moves</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/342/hong-kong</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/36616/qyshinsu-mystery-way</t>
+  </si>
+  <si>
+    <t>Qyshinsu</t>
+  </si>
+  <si>
+    <t>Bunte Runde</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/20122/bunte-runde</t>
+  </si>
+  <si>
+    <t>Attila</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/171663/attila</t>
+  </si>
+  <si>
+    <t>22 apples</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/38499/22-pommes</t>
+  </si>
+  <si>
+    <t>Taiga</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/86542/taiga</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>Dragon Lance</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/2836/dragon-lance-mage-stones</t>
+  </si>
+  <si>
+    <t>Rolling Village</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/306494/rolling-village</t>
+  </si>
+  <si>
+    <t>pnp, simple</t>
+  </si>
+  <si>
+    <t>Rove</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/342562/rove-results-oriented-versatile-explorer</t>
+  </si>
+  <si>
+    <t>pnp, check</t>
+  </si>
+  <si>
+    <t>Dig</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/197178/dig</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/90050/eleminis</t>
+  </si>
+  <si>
+    <t>Eleminis</t>
+  </si>
+  <si>
+    <t>Stoplights</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/29582/stoplights</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/40801/docker</t>
+  </si>
+  <si>
+    <t>Simple!</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/138748/flash</t>
+  </si>
+  <si>
+    <t>Shooting party</t>
+  </si>
+  <si>
+    <t>Solitaire; harder rules?</t>
+  </si>
+  <si>
+    <t>Ambagibus</t>
+  </si>
+  <si>
+    <t>https://boardgamegeek.com/boardgame/42498/ambagibus</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1694,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2497,6 +2662,12 @@
       <c r="I21" t="s">
         <v>196</v>
       </c>
+      <c r="J21" t="s">
+        <v>191</v>
+      </c>
+      <c r="K21" t="s">
+        <v>190</v>
+      </c>
       <c r="N21" t="str">
         <f t="shared" si="0"/>
         <v>3190/quixo</v>
@@ -2507,7 +2678,7 @@
       </c>
       <c r="P21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2D Arrays, Algorithms+</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -2526,8 +2697,8 @@
       <c r="E22">
         <v>7.4</v>
       </c>
-      <c r="F22" t="s">
-        <v>256</v>
+      <c r="F22">
+        <v>200</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>91</v>
@@ -2542,7 +2713,7 @@
         <v>191</v>
       </c>
       <c r="K22" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="0"/>
@@ -2554,7 +2725,7 @@
       </c>
       <c r="P22" t="str">
         <f t="shared" si="2"/>
-        <v>2D Arrays, Algorithms+</v>
+        <v>2D Arrays, Graphs</v>
       </c>
     </row>
   </sheetData>
@@ -2563,7 +2734,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8 G10:G12" xr:uid="{85B095F8-E867-4907-8DD0-AF461A936D35}">
       <formula1>"Low,High"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:L11 J12:K14" xr:uid="{80DF18E4-CD06-4E48-8072-6915464D3172}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J12:J14 J2:J11 L2:L11 K2:K22" xr:uid="{80DF18E4-CD06-4E48-8072-6915464D3172}">
       <formula1>Topics_Range</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I22" xr:uid="{3AED5C13-23B2-4C95-8785-73682780D1DB}">
@@ -2613,10 +2784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A9A40E-25F0-458E-A251-DF2D64A47FEF}">
-  <dimension ref="A1:N122"/>
+  <dimension ref="A1:N148"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3820,6 +3991,239 @@
       <c r="B122" s="1" t="s">
         <v>349</v>
       </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>350</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>352</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>353</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>356</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>358</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>360</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>362</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>364</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="K130" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L130" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>367</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>369</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>372</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>373</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="K134" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L134" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>375</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>377</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>379</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="L137" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>382</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>384</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K139" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L139" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>387</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="L140" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>390</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>393</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>394</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>396</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="L144" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>399</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="L145" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>401</v>
+      </c>
+      <c r="L146" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>403</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B148" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3914,9 +4318,30 @@
     <hyperlink ref="B119" r:id="rId89" xr:uid="{5067CC59-E44B-4C73-BEEB-A95B546DAE67}"/>
     <hyperlink ref="B121" r:id="rId90" xr:uid="{3C7A2F02-7B9A-4F21-957A-F9366874C5E0}"/>
     <hyperlink ref="B122" r:id="rId91" xr:uid="{C1DE438E-1F0F-400B-885D-DC268DC8B20C}"/>
+    <hyperlink ref="B123" r:id="rId92" xr:uid="{C2C460A9-CA95-41B0-8E8E-B476E345FAE2}"/>
+    <hyperlink ref="B126" r:id="rId93" xr:uid="{FCC488B5-3F44-4539-8530-14F1BF49887A}"/>
+    <hyperlink ref="B127" r:id="rId94" xr:uid="{9F08665E-D873-49E2-912F-AE7448FED47F}"/>
+    <hyperlink ref="B128" r:id="rId95" xr:uid="{3ECF1FB2-EEBB-4E7C-8C3E-E71336F63B6D}"/>
+    <hyperlink ref="B129" r:id="rId96" xr:uid="{6B014460-56A2-4EBB-957B-CD72E69C2C26}"/>
+    <hyperlink ref="B130" r:id="rId97" xr:uid="{E5FF010D-5C5F-40E2-982C-460D14AD52E7}"/>
+    <hyperlink ref="B131" r:id="rId98" xr:uid="{E1966F4E-B808-4A28-8105-78B4F17EA587}"/>
+    <hyperlink ref="B132" r:id="rId99" xr:uid="{5FF7748A-47F4-4A68-9268-59AB89771BAF}"/>
+    <hyperlink ref="B133" r:id="rId100" xr:uid="{D4D65006-1D97-4BA2-9EDB-12D4A5C411E6}"/>
+    <hyperlink ref="B134" r:id="rId101" xr:uid="{D0BA6B8E-F5A2-40C4-B53B-860625868A20}"/>
+    <hyperlink ref="B135" r:id="rId102" xr:uid="{57B28CDA-B5DB-425F-A450-4C10471EDE8B}"/>
+    <hyperlink ref="B136" r:id="rId103" xr:uid="{51E049C2-FBA4-436A-A84E-8BE790CB4494}"/>
+    <hyperlink ref="B137" r:id="rId104" xr:uid="{C4B91E9A-6D0E-4643-84BC-7BA38A5D86F8}"/>
+    <hyperlink ref="B138" r:id="rId105" xr:uid="{3B446812-02A2-4CE3-ACF9-50842D64FFC9}"/>
+    <hyperlink ref="B140" r:id="rId106" xr:uid="{7F58B1D8-ED81-4CDC-8A58-042DD95DEE54}"/>
+    <hyperlink ref="B141" r:id="rId107" xr:uid="{4713D2A2-CBBE-40C5-81ED-3628DA0624E5}"/>
+    <hyperlink ref="B142" r:id="rId108" xr:uid="{59F61A43-9688-46FF-B24E-FF5294A2FFDB}"/>
+    <hyperlink ref="B143" r:id="rId109" xr:uid="{5E98B109-8AEC-4739-A1A8-0E122D5A461A}"/>
+    <hyperlink ref="B144" r:id="rId110" xr:uid="{DFE88DE8-5BA8-4633-9F74-503A70048C4D}"/>
+    <hyperlink ref="B145" r:id="rId111" xr:uid="{010EAF79-16A6-4E33-AAFE-7EC0FBD40572}"/>
+    <hyperlink ref="B147" r:id="rId112" xr:uid="{C5A747F1-3BDD-4096-8005-2238182729D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId92"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId113"/>
 </worksheet>
 </file>
 
@@ -3924,9 +4349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EA451C-327E-4513-9273-EE648987230B}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView topLeftCell="A1048548" workbookViewId="0">
-      <selection activeCell="A1048576" sqref="A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>